<commit_message>
Minor changes to menu output formatting
</commit_message>
<xml_diff>
--- a/week2/UiPath_ExcelAutomationExercise/Menu.xlsx
+++ b/week2/UiPath_ExcelAutomationExercise/Menu.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\gavin-gilbert-code\week2\UiPath_ExcelAutomationExercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDE158B-2726-4545-91D6-067609A2DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{34898BFB-414F-4CE8-B93D-185338726C6E}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Menu" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46E168-A907-486D-A6BC-148DB3939B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34898BFB-414F-4CE8-B93D-185338726C6E}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Menu" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -31,107 +30,95 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <x:si>
-    <x:t>Dish Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chef's Special</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Valentine's Exclusive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ratatouille</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Monte Cristo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Love Boat</x:t>
-  </x:si>
-  <x:si>
-    <x:t>John Petrucci</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Dish Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Chef's Special</t>
+  </si>
+  <si>
+    <t>Valentine's Exclusive</t>
+  </si>
+  <si>
+    <t>Ratatouille</t>
+  </si>
+  <si>
+    <t>Monte Cristo</t>
+  </si>
+  <si>
+    <t>Love Boat</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="4">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,102 +417,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{F993D65F-CF92-4212-9361-B76558833E20}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D9"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G18" sqref="G18"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="13.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="13.570312" style="2" customWidth="1"/>
-    <x:col min="4" max="4" width="20.570312" style="2" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="n">
-        <x:v>22.99</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D2" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="n">
-        <x:v>18.99</x:v>
-      </x:c>
-      <x:c r="C3" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D3" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="n">
-        <x:v>13.99</x:v>
-      </x:c>
-      <x:c r="C4" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D4" s="2" t="b">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="A5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" s="1" t="n">
-        <x:v>99.99</x:v>
-      </x:c>
-      <x:c r="C5" s="2" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D5" s="2" t="b">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="C9" s="0" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F993D65F-CF92-4212-9361-B76558833E20}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="A5:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22.99</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>13.99</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>